<commit_message>
correction d'une erreur dans le plan de test
</commit_message>
<xml_diff>
--- a/Plan_de_tests.xlsx
+++ b/Plan_de_tests.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Lignes de code testées</t>
   </si>
   <si>
-    <t xml:space="preserve">Fonction testée</t>
+    <t xml:space="preserve">Élément testé</t>
   </si>
   <si>
     <t xml:space="preserve">Résultat attendu</t>
@@ -118,23 +118,7 @@
     <t xml:space="preserve">Variables « myHTML » et « HTML »</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Création du HTML dans « myHTML » pour chaque article avec variables pour l’image, le nom, le prix et l’id dans le lien. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Initialisation du HTML dans la page</t>
-    </r>
+    <t xml:space="preserve">Création du HTML dans « myHTML » pour chaque article avec variables pour l’image, le nom, le prix et l’id dans le lien. Initialisation du HTML dans la page</t>
   </si>
   <si>
     <t xml:space="preserve">Actualiser la page</t>
@@ -483,7 +467,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -525,17 +509,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -617,7 +590,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -686,14 +659,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -707,10 +672,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -804,10 +765,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.12"/>
@@ -1292,10 +1253,10 @@
       <c r="C24" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="17" t="s">
+      <c r="D24" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="16" t="s">
         <v>107</v>
       </c>
       <c r="F24" s="16" t="s">
@@ -1383,82 +1344,82 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="20" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F30" s="20" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D31" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="20" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B32" s="20" t="n">
+      <c r="B32" s="18" t="n">
         <v>51</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="20" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1481,1124 +1442,1124 @@
     <row r="49" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="50" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
     </row>
     <row r="52" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
     </row>
     <row r="53" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="24"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
     </row>
     <row r="54" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
     </row>
     <row r="55" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="24"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="22"/>
     </row>
     <row r="56" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="24"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
+      <c r="A56" s="21"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
     </row>
     <row r="57" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="24"/>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
     </row>
     <row r="58" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
     </row>
     <row r="59" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="24"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
+      <c r="F59" s="22"/>
     </row>
     <row r="60" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="24"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
     </row>
     <row r="61" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="24"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="22"/>
     </row>
     <row r="62" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="24"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="22"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="24"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="22"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="24"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
+      <c r="A64" s="21"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="22"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="24"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
+      <c r="A65" s="21"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="24"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="22"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="24"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="22"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="24"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
+      <c r="A68" s="21"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="22"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="24"/>
-      <c r="B69" s="24"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
+      <c r="A69" s="21"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="24"/>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="24"/>
-      <c r="B71" s="24"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="24"/>
-      <c r="B72" s="24"/>
-      <c r="C72" s="24"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="22"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="24"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="24"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="22"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="24"/>
-      <c r="B74" s="24"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
+      <c r="A74" s="21"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="21"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="22"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="24"/>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="25"/>
+      <c r="A75" s="21"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="22"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="24"/>
-      <c r="B76" s="24"/>
-      <c r="C76" s="24"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
+      <c r="A76" s="21"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="24"/>
-      <c r="B77" s="24"/>
-      <c r="C77" s="24"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
+      <c r="A77" s="21"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
+      <c r="F77" s="22"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="24"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
+      <c r="A78" s="21"/>
+      <c r="B78" s="21"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="22"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="24"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="24"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="22"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="24"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="25"/>
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="22"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="24"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="24"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="25"/>
-      <c r="F82" s="25"/>
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="22"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="24"/>
-      <c r="B83" s="24"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="25"/>
-      <c r="E83" s="25"/>
-      <c r="F83" s="25"/>
+      <c r="A83" s="21"/>
+      <c r="B83" s="21"/>
+      <c r="C83" s="21"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
+      <c r="F83" s="22"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="24"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="25"/>
-      <c r="F84" s="25"/>
+      <c r="A84" s="21"/>
+      <c r="B84" s="21"/>
+      <c r="C84" s="21"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
+      <c r="F84" s="22"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="24"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="25"/>
-      <c r="F85" s="25"/>
+      <c r="A85" s="21"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="24"/>
-      <c r="B86" s="24"/>
-      <c r="C86" s="24"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="25"/>
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="24"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="24"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
+      <c r="A87" s="21"/>
+      <c r="B87" s="21"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="22"/>
+      <c r="F87" s="22"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="24"/>
-      <c r="B88" s="24"/>
-      <c r="C88" s="24"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25"/>
+      <c r="A88" s="21"/>
+      <c r="B88" s="21"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="22"/>
+      <c r="F88" s="22"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="24"/>
-      <c r="B89" s="24"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="25"/>
-      <c r="E89" s="25"/>
-      <c r="F89" s="25"/>
+      <c r="A89" s="21"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="22"/>
+      <c r="F89" s="22"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="24"/>
-      <c r="B90" s="24"/>
-      <c r="C90" s="24"/>
-      <c r="D90" s="25"/>
-      <c r="E90" s="25"/>
-      <c r="F90" s="25"/>
+      <c r="A90" s="21"/>
+      <c r="B90" s="21"/>
+      <c r="C90" s="21"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="22"/>
+      <c r="F90" s="22"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="24"/>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
+      <c r="A91" s="21"/>
+      <c r="B91" s="21"/>
+      <c r="C91" s="21"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="22"/>
+      <c r="F91" s="22"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="24"/>
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
-      <c r="D92" s="25"/>
-      <c r="E92" s="25"/>
-      <c r="F92" s="25"/>
+      <c r="A92" s="21"/>
+      <c r="B92" s="21"/>
+      <c r="C92" s="21"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="22"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="24"/>
-      <c r="B93" s="24"/>
-      <c r="C93" s="24"/>
-      <c r="D93" s="25"/>
-      <c r="E93" s="25"/>
-      <c r="F93" s="25"/>
+      <c r="A93" s="21"/>
+      <c r="B93" s="21"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="22"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="24"/>
-      <c r="B94" s="24"/>
-      <c r="C94" s="24"/>
-      <c r="D94" s="25"/>
-      <c r="E94" s="25"/>
-      <c r="F94" s="25"/>
+      <c r="A94" s="21"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="22"/>
+      <c r="E94" s="22"/>
+      <c r="F94" s="22"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="24"/>
-      <c r="B95" s="24"/>
-      <c r="C95" s="24"/>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="25"/>
+      <c r="A95" s="21"/>
+      <c r="B95" s="21"/>
+      <c r="C95" s="21"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="22"/>
+      <c r="F95" s="22"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="24"/>
-      <c r="B96" s="24"/>
-      <c r="C96" s="24"/>
-      <c r="D96" s="25"/>
-      <c r="E96" s="25"/>
-      <c r="F96" s="25"/>
+      <c r="A96" s="21"/>
+      <c r="B96" s="21"/>
+      <c r="C96" s="21"/>
+      <c r="D96" s="22"/>
+      <c r="E96" s="22"/>
+      <c r="F96" s="22"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="24"/>
-      <c r="B97" s="24"/>
-      <c r="C97" s="24"/>
-      <c r="D97" s="25"/>
-      <c r="E97" s="25"/>
-      <c r="F97" s="25"/>
+      <c r="A97" s="21"/>
+      <c r="B97" s="21"/>
+      <c r="C97" s="21"/>
+      <c r="D97" s="22"/>
+      <c r="E97" s="22"/>
+      <c r="F97" s="22"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="24"/>
-      <c r="B98" s="24"/>
-      <c r="C98" s="24"/>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
+      <c r="A98" s="21"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="21"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="22"/>
+      <c r="F98" s="22"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="24"/>
-      <c r="B99" s="24"/>
-      <c r="C99" s="24"/>
-      <c r="D99" s="25"/>
-      <c r="E99" s="25"/>
-      <c r="F99" s="25"/>
+      <c r="A99" s="21"/>
+      <c r="B99" s="21"/>
+      <c r="C99" s="21"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="22"/>
+      <c r="F99" s="22"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="24"/>
-      <c r="B100" s="24"/>
-      <c r="C100" s="24"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
+      <c r="A100" s="21"/>
+      <c r="B100" s="21"/>
+      <c r="C100" s="21"/>
+      <c r="D100" s="22"/>
+      <c r="E100" s="22"/>
+      <c r="F100" s="22"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="24"/>
-      <c r="B101" s="24"/>
-      <c r="C101" s="24"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="25"/>
+      <c r="A101" s="21"/>
+      <c r="B101" s="21"/>
+      <c r="C101" s="21"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="22"/>
+      <c r="F101" s="22"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="24"/>
-      <c r="B102" s="24"/>
-      <c r="C102" s="24"/>
-      <c r="D102" s="25"/>
-      <c r="E102" s="25"/>
-      <c r="F102" s="25"/>
+      <c r="A102" s="21"/>
+      <c r="B102" s="21"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="22"/>
+      <c r="E102" s="22"/>
+      <c r="F102" s="22"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="24"/>
-      <c r="B103" s="24"/>
-      <c r="C103" s="24"/>
-      <c r="D103" s="25"/>
-      <c r="E103" s="25"/>
-      <c r="F103" s="25"/>
+      <c r="A103" s="21"/>
+      <c r="B103" s="21"/>
+      <c r="C103" s="21"/>
+      <c r="D103" s="22"/>
+      <c r="E103" s="22"/>
+      <c r="F103" s="22"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="24"/>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24"/>
-      <c r="D104" s="25"/>
-      <c r="E104" s="25"/>
-      <c r="F104" s="25"/>
+      <c r="A104" s="21"/>
+      <c r="B104" s="21"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="22"/>
+      <c r="E104" s="22"/>
+      <c r="F104" s="22"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="24"/>
-      <c r="B105" s="24"/>
-      <c r="C105" s="24"/>
-      <c r="D105" s="25"/>
-      <c r="E105" s="25"/>
-      <c r="F105" s="25"/>
+      <c r="A105" s="21"/>
+      <c r="B105" s="21"/>
+      <c r="C105" s="21"/>
+      <c r="D105" s="22"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="22"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="24"/>
-      <c r="B106" s="24"/>
-      <c r="C106" s="24"/>
-      <c r="D106" s="25"/>
-      <c r="E106" s="25"/>
-      <c r="F106" s="25"/>
+      <c r="A106" s="21"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="21"/>
+      <c r="D106" s="22"/>
+      <c r="E106" s="22"/>
+      <c r="F106" s="22"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="24"/>
-      <c r="B107" s="24"/>
-      <c r="C107" s="24"/>
-      <c r="D107" s="25"/>
-      <c r="E107" s="25"/>
-      <c r="F107" s="25"/>
+      <c r="A107" s="21"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="22"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="22"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="24"/>
-      <c r="B108" s="24"/>
-      <c r="C108" s="24"/>
-      <c r="D108" s="25"/>
-      <c r="E108" s="25"/>
-      <c r="F108" s="25"/>
+      <c r="A108" s="21"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="21"/>
+      <c r="D108" s="22"/>
+      <c r="E108" s="22"/>
+      <c r="F108" s="22"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="24"/>
-      <c r="B109" s="24"/>
-      <c r="C109" s="24"/>
-      <c r="D109" s="25"/>
-      <c r="E109" s="25"/>
-      <c r="F109" s="25"/>
+      <c r="A109" s="21"/>
+      <c r="B109" s="21"/>
+      <c r="C109" s="21"/>
+      <c r="D109" s="22"/>
+      <c r="E109" s="22"/>
+      <c r="F109" s="22"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="24"/>
-      <c r="B110" s="24"/>
-      <c r="C110" s="24"/>
-      <c r="D110" s="25"/>
-      <c r="E110" s="25"/>
-      <c r="F110" s="25"/>
+      <c r="A110" s="21"/>
+      <c r="B110" s="21"/>
+      <c r="C110" s="21"/>
+      <c r="D110" s="22"/>
+      <c r="E110" s="22"/>
+      <c r="F110" s="22"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="24"/>
-      <c r="B111" s="24"/>
-      <c r="C111" s="24"/>
-      <c r="D111" s="25"/>
-      <c r="E111" s="25"/>
-      <c r="F111" s="25"/>
+      <c r="A111" s="21"/>
+      <c r="B111" s="21"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="22"/>
+      <c r="E111" s="22"/>
+      <c r="F111" s="22"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="24"/>
-      <c r="B112" s="24"/>
-      <c r="C112" s="24"/>
-      <c r="D112" s="25"/>
-      <c r="E112" s="25"/>
-      <c r="F112" s="25"/>
+      <c r="A112" s="21"/>
+      <c r="B112" s="21"/>
+      <c r="C112" s="21"/>
+      <c r="D112" s="22"/>
+      <c r="E112" s="22"/>
+      <c r="F112" s="22"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="24"/>
-      <c r="B113" s="24"/>
-      <c r="C113" s="24"/>
-      <c r="D113" s="25"/>
-      <c r="E113" s="25"/>
-      <c r="F113" s="25"/>
+      <c r="A113" s="21"/>
+      <c r="B113" s="21"/>
+      <c r="C113" s="21"/>
+      <c r="D113" s="22"/>
+      <c r="E113" s="22"/>
+      <c r="F113" s="22"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="24"/>
-      <c r="B114" s="24"/>
-      <c r="C114" s="24"/>
-      <c r="D114" s="25"/>
-      <c r="E114" s="25"/>
-      <c r="F114" s="25"/>
+      <c r="A114" s="21"/>
+      <c r="B114" s="21"/>
+      <c r="C114" s="21"/>
+      <c r="D114" s="22"/>
+      <c r="E114" s="22"/>
+      <c r="F114" s="22"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="24"/>
-      <c r="B115" s="24"/>
-      <c r="C115" s="24"/>
-      <c r="D115" s="25"/>
-      <c r="E115" s="25"/>
-      <c r="F115" s="25"/>
+      <c r="A115" s="21"/>
+      <c r="B115" s="21"/>
+      <c r="C115" s="21"/>
+      <c r="D115" s="22"/>
+      <c r="E115" s="22"/>
+      <c r="F115" s="22"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="24"/>
-      <c r="B116" s="24"/>
-      <c r="C116" s="24"/>
-      <c r="D116" s="25"/>
-      <c r="E116" s="25"/>
-      <c r="F116" s="25"/>
+      <c r="A116" s="21"/>
+      <c r="B116" s="21"/>
+      <c r="C116" s="21"/>
+      <c r="D116" s="22"/>
+      <c r="E116" s="22"/>
+      <c r="F116" s="22"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="24"/>
-      <c r="B117" s="24"/>
-      <c r="C117" s="24"/>
-      <c r="D117" s="25"/>
-      <c r="E117" s="25"/>
-      <c r="F117" s="25"/>
+      <c r="A117" s="21"/>
+      <c r="B117" s="21"/>
+      <c r="C117" s="21"/>
+      <c r="D117" s="22"/>
+      <c r="E117" s="22"/>
+      <c r="F117" s="22"/>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="24"/>
-      <c r="B118" s="24"/>
-      <c r="C118" s="24"/>
-      <c r="D118" s="25"/>
-      <c r="E118" s="25"/>
-      <c r="F118" s="25"/>
+      <c r="A118" s="21"/>
+      <c r="B118" s="21"/>
+      <c r="C118" s="21"/>
+      <c r="D118" s="22"/>
+      <c r="E118" s="22"/>
+      <c r="F118" s="22"/>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="24"/>
-      <c r="B119" s="24"/>
-      <c r="C119" s="24"/>
-      <c r="D119" s="25"/>
-      <c r="E119" s="25"/>
-      <c r="F119" s="25"/>
+      <c r="A119" s="21"/>
+      <c r="B119" s="21"/>
+      <c r="C119" s="21"/>
+      <c r="D119" s="22"/>
+      <c r="E119" s="22"/>
+      <c r="F119" s="22"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="24"/>
-      <c r="B120" s="24"/>
-      <c r="C120" s="24"/>
-      <c r="D120" s="25"/>
-      <c r="E120" s="25"/>
-      <c r="F120" s="25"/>
+      <c r="A120" s="21"/>
+      <c r="B120" s="21"/>
+      <c r="C120" s="21"/>
+      <c r="D120" s="22"/>
+      <c r="E120" s="22"/>
+      <c r="F120" s="22"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="24"/>
-      <c r="B121" s="24"/>
-      <c r="C121" s="24"/>
-      <c r="D121" s="25"/>
-      <c r="E121" s="25"/>
-      <c r="F121" s="25"/>
+      <c r="A121" s="21"/>
+      <c r="B121" s="21"/>
+      <c r="C121" s="21"/>
+      <c r="D121" s="22"/>
+      <c r="E121" s="22"/>
+      <c r="F121" s="22"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="24"/>
-      <c r="B122" s="24"/>
-      <c r="C122" s="24"/>
-      <c r="D122" s="25"/>
-      <c r="E122" s="25"/>
-      <c r="F122" s="25"/>
+      <c r="A122" s="21"/>
+      <c r="B122" s="21"/>
+      <c r="C122" s="21"/>
+      <c r="D122" s="22"/>
+      <c r="E122" s="22"/>
+      <c r="F122" s="22"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="24"/>
-      <c r="B123" s="24"/>
-      <c r="C123" s="24"/>
-      <c r="D123" s="25"/>
-      <c r="E123" s="25"/>
-      <c r="F123" s="25"/>
+      <c r="A123" s="21"/>
+      <c r="B123" s="21"/>
+      <c r="C123" s="21"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="22"/>
+      <c r="F123" s="22"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="24"/>
-      <c r="B124" s="24"/>
-      <c r="C124" s="24"/>
-      <c r="D124" s="25"/>
-      <c r="E124" s="25"/>
-      <c r="F124" s="25"/>
+      <c r="A124" s="21"/>
+      <c r="B124" s="21"/>
+      <c r="C124" s="21"/>
+      <c r="D124" s="22"/>
+      <c r="E124" s="22"/>
+      <c r="F124" s="22"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="24"/>
-      <c r="B125" s="24"/>
-      <c r="C125" s="24"/>
-      <c r="D125" s="25"/>
-      <c r="E125" s="25"/>
-      <c r="F125" s="25"/>
+      <c r="A125" s="21"/>
+      <c r="B125" s="21"/>
+      <c r="C125" s="21"/>
+      <c r="D125" s="22"/>
+      <c r="E125" s="22"/>
+      <c r="F125" s="22"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="24"/>
-      <c r="B126" s="24"/>
-      <c r="C126" s="24"/>
-      <c r="D126" s="25"/>
-      <c r="E126" s="25"/>
-      <c r="F126" s="25"/>
+      <c r="A126" s="21"/>
+      <c r="B126" s="21"/>
+      <c r="C126" s="21"/>
+      <c r="D126" s="22"/>
+      <c r="E126" s="22"/>
+      <c r="F126" s="22"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="24"/>
-      <c r="B127" s="24"/>
-      <c r="C127" s="24"/>
-      <c r="D127" s="25"/>
-      <c r="E127" s="25"/>
-      <c r="F127" s="25"/>
+      <c r="A127" s="21"/>
+      <c r="B127" s="21"/>
+      <c r="C127" s="21"/>
+      <c r="D127" s="22"/>
+      <c r="E127" s="22"/>
+      <c r="F127" s="22"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="24"/>
-      <c r="B128" s="24"/>
-      <c r="C128" s="24"/>
-      <c r="D128" s="25"/>
-      <c r="E128" s="25"/>
-      <c r="F128" s="25"/>
+      <c r="A128" s="21"/>
+      <c r="B128" s="21"/>
+      <c r="C128" s="21"/>
+      <c r="D128" s="22"/>
+      <c r="E128" s="22"/>
+      <c r="F128" s="22"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="24"/>
-      <c r="B129" s="24"/>
-      <c r="C129" s="24"/>
-      <c r="D129" s="25"/>
-      <c r="E129" s="25"/>
-      <c r="F129" s="25"/>
+      <c r="A129" s="21"/>
+      <c r="B129" s="21"/>
+      <c r="C129" s="21"/>
+      <c r="D129" s="22"/>
+      <c r="E129" s="22"/>
+      <c r="F129" s="22"/>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="24"/>
-      <c r="B130" s="24"/>
-      <c r="C130" s="24"/>
-      <c r="D130" s="25"/>
-      <c r="E130" s="25"/>
-      <c r="F130" s="25"/>
+      <c r="A130" s="21"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="21"/>
+      <c r="D130" s="22"/>
+      <c r="E130" s="22"/>
+      <c r="F130" s="22"/>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="24"/>
-      <c r="B131" s="24"/>
-      <c r="C131" s="24"/>
-      <c r="D131" s="25"/>
-      <c r="E131" s="25"/>
-      <c r="F131" s="25"/>
+      <c r="A131" s="21"/>
+      <c r="B131" s="21"/>
+      <c r="C131" s="21"/>
+      <c r="D131" s="22"/>
+      <c r="E131" s="22"/>
+      <c r="F131" s="22"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="24"/>
-      <c r="B132" s="24"/>
-      <c r="C132" s="24"/>
-      <c r="D132" s="25"/>
-      <c r="E132" s="25"/>
-      <c r="F132" s="25"/>
+      <c r="A132" s="21"/>
+      <c r="B132" s="21"/>
+      <c r="C132" s="21"/>
+      <c r="D132" s="22"/>
+      <c r="E132" s="22"/>
+      <c r="F132" s="22"/>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="24"/>
-      <c r="B133" s="24"/>
-      <c r="C133" s="24"/>
-      <c r="D133" s="25"/>
-      <c r="E133" s="25"/>
-      <c r="F133" s="25"/>
+      <c r="A133" s="21"/>
+      <c r="B133" s="21"/>
+      <c r="C133" s="21"/>
+      <c r="D133" s="22"/>
+      <c r="E133" s="22"/>
+      <c r="F133" s="22"/>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="24"/>
-      <c r="B134" s="24"/>
-      <c r="C134" s="24"/>
-      <c r="D134" s="25"/>
-      <c r="E134" s="25"/>
-      <c r="F134" s="25"/>
+      <c r="A134" s="21"/>
+      <c r="B134" s="21"/>
+      <c r="C134" s="21"/>
+      <c r="D134" s="22"/>
+      <c r="E134" s="22"/>
+      <c r="F134" s="22"/>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="24"/>
-      <c r="B135" s="24"/>
-      <c r="C135" s="24"/>
-      <c r="D135" s="25"/>
-      <c r="E135" s="25"/>
-      <c r="F135" s="25"/>
+      <c r="A135" s="21"/>
+      <c r="B135" s="21"/>
+      <c r="C135" s="21"/>
+      <c r="D135" s="22"/>
+      <c r="E135" s="22"/>
+      <c r="F135" s="22"/>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="24"/>
-      <c r="B136" s="24"/>
-      <c r="C136" s="24"/>
-      <c r="D136" s="25"/>
-      <c r="E136" s="25"/>
-      <c r="F136" s="25"/>
+      <c r="A136" s="21"/>
+      <c r="B136" s="21"/>
+      <c r="C136" s="21"/>
+      <c r="D136" s="22"/>
+      <c r="E136" s="22"/>
+      <c r="F136" s="22"/>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="24"/>
-      <c r="B137" s="24"/>
-      <c r="C137" s="24"/>
-      <c r="D137" s="25"/>
-      <c r="E137" s="25"/>
-      <c r="F137" s="25"/>
+      <c r="A137" s="21"/>
+      <c r="B137" s="21"/>
+      <c r="C137" s="21"/>
+      <c r="D137" s="22"/>
+      <c r="E137" s="22"/>
+      <c r="F137" s="22"/>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="24"/>
-      <c r="B138" s="24"/>
-      <c r="C138" s="24"/>
-      <c r="D138" s="25"/>
-      <c r="E138" s="25"/>
-      <c r="F138" s="25"/>
+      <c r="A138" s="21"/>
+      <c r="B138" s="21"/>
+      <c r="C138" s="21"/>
+      <c r="D138" s="22"/>
+      <c r="E138" s="22"/>
+      <c r="F138" s="22"/>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="24"/>
-      <c r="B139" s="24"/>
-      <c r="C139" s="24"/>
-      <c r="D139" s="25"/>
-      <c r="E139" s="25"/>
-      <c r="F139" s="25"/>
+      <c r="A139" s="21"/>
+      <c r="B139" s="21"/>
+      <c r="C139" s="21"/>
+      <c r="D139" s="22"/>
+      <c r="E139" s="22"/>
+      <c r="F139" s="22"/>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="24"/>
-      <c r="B140" s="24"/>
-      <c r="C140" s="24"/>
-      <c r="D140" s="25"/>
-      <c r="E140" s="25"/>
-      <c r="F140" s="25"/>
+      <c r="A140" s="21"/>
+      <c r="B140" s="21"/>
+      <c r="C140" s="21"/>
+      <c r="D140" s="22"/>
+      <c r="E140" s="22"/>
+      <c r="F140" s="22"/>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="24"/>
-      <c r="B141" s="24"/>
-      <c r="C141" s="24"/>
-      <c r="D141" s="25"/>
-      <c r="E141" s="25"/>
-      <c r="F141" s="25"/>
+      <c r="A141" s="21"/>
+      <c r="B141" s="21"/>
+      <c r="C141" s="21"/>
+      <c r="D141" s="22"/>
+      <c r="E141" s="22"/>
+      <c r="F141" s="22"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="24"/>
-      <c r="B142" s="24"/>
-      <c r="C142" s="24"/>
-      <c r="D142" s="25"/>
-      <c r="E142" s="25"/>
-      <c r="F142" s="25"/>
+      <c r="A142" s="21"/>
+      <c r="B142" s="21"/>
+      <c r="C142" s="21"/>
+      <c r="D142" s="22"/>
+      <c r="E142" s="22"/>
+      <c r="F142" s="22"/>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="24"/>
-      <c r="B143" s="24"/>
-      <c r="C143" s="24"/>
-      <c r="D143" s="25"/>
-      <c r="E143" s="25"/>
-      <c r="F143" s="25"/>
+      <c r="A143" s="21"/>
+      <c r="B143" s="21"/>
+      <c r="C143" s="21"/>
+      <c r="D143" s="22"/>
+      <c r="E143" s="22"/>
+      <c r="F143" s="22"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="24"/>
-      <c r="B144" s="24"/>
-      <c r="C144" s="24"/>
-      <c r="D144" s="25"/>
-      <c r="E144" s="25"/>
-      <c r="F144" s="25"/>
+      <c r="A144" s="21"/>
+      <c r="B144" s="21"/>
+      <c r="C144" s="21"/>
+      <c r="D144" s="22"/>
+      <c r="E144" s="22"/>
+      <c r="F144" s="22"/>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="24"/>
-      <c r="B145" s="24"/>
-      <c r="C145" s="24"/>
-      <c r="D145" s="25"/>
-      <c r="E145" s="25"/>
-      <c r="F145" s="25"/>
+      <c r="A145" s="21"/>
+      <c r="B145" s="21"/>
+      <c r="C145" s="21"/>
+      <c r="D145" s="22"/>
+      <c r="E145" s="22"/>
+      <c r="F145" s="22"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="24"/>
-      <c r="B146" s="24"/>
-      <c r="C146" s="24"/>
-      <c r="D146" s="25"/>
-      <c r="E146" s="25"/>
-      <c r="F146" s="25"/>
+      <c r="A146" s="21"/>
+      <c r="B146" s="21"/>
+      <c r="C146" s="21"/>
+      <c r="D146" s="22"/>
+      <c r="E146" s="22"/>
+      <c r="F146" s="22"/>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="24"/>
-      <c r="B147" s="24"/>
-      <c r="C147" s="24"/>
-      <c r="D147" s="25"/>
-      <c r="E147" s="25"/>
-      <c r="F147" s="25"/>
+      <c r="A147" s="21"/>
+      <c r="B147" s="21"/>
+      <c r="C147" s="21"/>
+      <c r="D147" s="22"/>
+      <c r="E147" s="22"/>
+      <c r="F147" s="22"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="24"/>
-      <c r="B148" s="24"/>
-      <c r="C148" s="24"/>
-      <c r="D148" s="25"/>
-      <c r="E148" s="25"/>
-      <c r="F148" s="25"/>
+      <c r="A148" s="21"/>
+      <c r="B148" s="21"/>
+      <c r="C148" s="21"/>
+      <c r="D148" s="22"/>
+      <c r="E148" s="22"/>
+      <c r="F148" s="22"/>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="24"/>
-      <c r="B149" s="24"/>
-      <c r="C149" s="24"/>
-      <c r="D149" s="25"/>
-      <c r="E149" s="25"/>
-      <c r="F149" s="25"/>
+      <c r="A149" s="21"/>
+      <c r="B149" s="21"/>
+      <c r="C149" s="21"/>
+      <c r="D149" s="22"/>
+      <c r="E149" s="22"/>
+      <c r="F149" s="22"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="24"/>
-      <c r="B150" s="24"/>
-      <c r="C150" s="24"/>
-      <c r="D150" s="25"/>
-      <c r="E150" s="25"/>
-      <c r="F150" s="25"/>
+      <c r="A150" s="21"/>
+      <c r="B150" s="21"/>
+      <c r="C150" s="21"/>
+      <c r="D150" s="22"/>
+      <c r="E150" s="22"/>
+      <c r="F150" s="22"/>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="24"/>
-      <c r="B151" s="24"/>
-      <c r="C151" s="24"/>
-      <c r="D151" s="25"/>
-      <c r="E151" s="25"/>
-      <c r="F151" s="25"/>
+      <c r="A151" s="21"/>
+      <c r="B151" s="21"/>
+      <c r="C151" s="21"/>
+      <c r="D151" s="22"/>
+      <c r="E151" s="22"/>
+      <c r="F151" s="22"/>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="24"/>
-      <c r="B152" s="24"/>
-      <c r="C152" s="24"/>
-      <c r="D152" s="25"/>
-      <c r="E152" s="25"/>
-      <c r="F152" s="25"/>
+      <c r="A152" s="21"/>
+      <c r="B152" s="21"/>
+      <c r="C152" s="21"/>
+      <c r="D152" s="22"/>
+      <c r="E152" s="22"/>
+      <c r="F152" s="22"/>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="24"/>
-      <c r="B153" s="24"/>
-      <c r="C153" s="24"/>
-      <c r="D153" s="25"/>
-      <c r="E153" s="25"/>
-      <c r="F153" s="25"/>
+      <c r="A153" s="21"/>
+      <c r="B153" s="21"/>
+      <c r="C153" s="21"/>
+      <c r="D153" s="22"/>
+      <c r="E153" s="22"/>
+      <c r="F153" s="22"/>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="24"/>
-      <c r="B154" s="24"/>
-      <c r="C154" s="24"/>
-      <c r="D154" s="25"/>
-      <c r="E154" s="25"/>
-      <c r="F154" s="25"/>
+      <c r="A154" s="21"/>
+      <c r="B154" s="21"/>
+      <c r="C154" s="21"/>
+      <c r="D154" s="22"/>
+      <c r="E154" s="22"/>
+      <c r="F154" s="22"/>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="24"/>
-      <c r="B155" s="24"/>
-      <c r="C155" s="24"/>
-      <c r="D155" s="25"/>
-      <c r="E155" s="25"/>
-      <c r="F155" s="25"/>
+      <c r="A155" s="21"/>
+      <c r="B155" s="21"/>
+      <c r="C155" s="21"/>
+      <c r="D155" s="22"/>
+      <c r="E155" s="22"/>
+      <c r="F155" s="22"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="24"/>
-      <c r="B156" s="24"/>
-      <c r="C156" s="24"/>
-      <c r="D156" s="25"/>
-      <c r="E156" s="25"/>
-      <c r="F156" s="25"/>
+      <c r="A156" s="21"/>
+      <c r="B156" s="21"/>
+      <c r="C156" s="21"/>
+      <c r="D156" s="22"/>
+      <c r="E156" s="22"/>
+      <c r="F156" s="22"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="24"/>
-      <c r="B157" s="24"/>
-      <c r="C157" s="24"/>
-      <c r="D157" s="25"/>
-      <c r="E157" s="25"/>
-      <c r="F157" s="25"/>
+      <c r="A157" s="21"/>
+      <c r="B157" s="21"/>
+      <c r="C157" s="21"/>
+      <c r="D157" s="22"/>
+      <c r="E157" s="22"/>
+      <c r="F157" s="22"/>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="24"/>
-      <c r="B158" s="24"/>
-      <c r="C158" s="24"/>
-      <c r="D158" s="25"/>
-      <c r="E158" s="25"/>
-      <c r="F158" s="25"/>
+      <c r="A158" s="21"/>
+      <c r="B158" s="21"/>
+      <c r="C158" s="21"/>
+      <c r="D158" s="22"/>
+      <c r="E158" s="22"/>
+      <c r="F158" s="22"/>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="24"/>
-      <c r="B159" s="24"/>
-      <c r="C159" s="24"/>
-      <c r="D159" s="25"/>
-      <c r="E159" s="25"/>
-      <c r="F159" s="25"/>
+      <c r="A159" s="21"/>
+      <c r="B159" s="21"/>
+      <c r="C159" s="21"/>
+      <c r="D159" s="22"/>
+      <c r="E159" s="22"/>
+      <c r="F159" s="22"/>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="24"/>
-      <c r="B160" s="24"/>
-      <c r="C160" s="24"/>
-      <c r="D160" s="25"/>
-      <c r="E160" s="25"/>
-      <c r="F160" s="25"/>
+      <c r="A160" s="21"/>
+      <c r="B160" s="21"/>
+      <c r="C160" s="21"/>
+      <c r="D160" s="22"/>
+      <c r="E160" s="22"/>
+      <c r="F160" s="22"/>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="24"/>
-      <c r="B161" s="24"/>
-      <c r="C161" s="24"/>
-      <c r="D161" s="25"/>
-      <c r="E161" s="25"/>
-      <c r="F161" s="25"/>
+      <c r="A161" s="21"/>
+      <c r="B161" s="21"/>
+      <c r="C161" s="21"/>
+      <c r="D161" s="22"/>
+      <c r="E161" s="22"/>
+      <c r="F161" s="22"/>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="24"/>
-      <c r="B162" s="24"/>
-      <c r="C162" s="24"/>
-      <c r="D162" s="25"/>
-      <c r="E162" s="25"/>
-      <c r="F162" s="25"/>
+      <c r="A162" s="21"/>
+      <c r="B162" s="21"/>
+      <c r="C162" s="21"/>
+      <c r="D162" s="22"/>
+      <c r="E162" s="22"/>
+      <c r="F162" s="22"/>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="24"/>
-      <c r="B163" s="24"/>
-      <c r="C163" s="24"/>
-      <c r="D163" s="25"/>
-      <c r="E163" s="25"/>
-      <c r="F163" s="25"/>
+      <c r="A163" s="21"/>
+      <c r="B163" s="21"/>
+      <c r="C163" s="21"/>
+      <c r="D163" s="22"/>
+      <c r="E163" s="22"/>
+      <c r="F163" s="22"/>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="24"/>
-      <c r="B164" s="24"/>
-      <c r="C164" s="24"/>
-      <c r="D164" s="25"/>
-      <c r="E164" s="25"/>
-      <c r="F164" s="25"/>
+      <c r="A164" s="21"/>
+      <c r="B164" s="21"/>
+      <c r="C164" s="21"/>
+      <c r="D164" s="22"/>
+      <c r="E164" s="22"/>
+      <c r="F164" s="22"/>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="24"/>
-      <c r="B165" s="24"/>
-      <c r="C165" s="24"/>
-      <c r="D165" s="25"/>
-      <c r="E165" s="25"/>
-      <c r="F165" s="25"/>
+      <c r="A165" s="21"/>
+      <c r="B165" s="21"/>
+      <c r="C165" s="21"/>
+      <c r="D165" s="22"/>
+      <c r="E165" s="22"/>
+      <c r="F165" s="22"/>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="24"/>
-      <c r="B166" s="24"/>
-      <c r="C166" s="24"/>
-      <c r="D166" s="25"/>
-      <c r="E166" s="25"/>
-      <c r="F166" s="25"/>
+      <c r="A166" s="21"/>
+      <c r="B166" s="21"/>
+      <c r="C166" s="21"/>
+      <c r="D166" s="22"/>
+      <c r="E166" s="22"/>
+      <c r="F166" s="22"/>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="24"/>
-      <c r="B167" s="24"/>
-      <c r="C167" s="24"/>
-      <c r="D167" s="25"/>
-      <c r="E167" s="25"/>
-      <c r="F167" s="25"/>
+      <c r="A167" s="21"/>
+      <c r="B167" s="21"/>
+      <c r="C167" s="21"/>
+      <c r="D167" s="22"/>
+      <c r="E167" s="22"/>
+      <c r="F167" s="22"/>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="24"/>
-      <c r="B168" s="24"/>
-      <c r="C168" s="24"/>
-      <c r="D168" s="25"/>
-      <c r="E168" s="25"/>
-      <c r="F168" s="25"/>
+      <c r="A168" s="21"/>
+      <c r="B168" s="21"/>
+      <c r="C168" s="21"/>
+      <c r="D168" s="22"/>
+      <c r="E168" s="22"/>
+      <c r="F168" s="22"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="24"/>
-      <c r="B169" s="24"/>
-      <c r="C169" s="24"/>
-      <c r="D169" s="25"/>
-      <c r="E169" s="25"/>
-      <c r="F169" s="25"/>
+      <c r="A169" s="21"/>
+      <c r="B169" s="21"/>
+      <c r="C169" s="21"/>
+      <c r="D169" s="22"/>
+      <c r="E169" s="22"/>
+      <c r="F169" s="22"/>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="24"/>
-      <c r="B170" s="24"/>
-      <c r="C170" s="24"/>
-      <c r="D170" s="25"/>
-      <c r="E170" s="25"/>
-      <c r="F170" s="25"/>
+      <c r="A170" s="21"/>
+      <c r="B170" s="21"/>
+      <c r="C170" s="21"/>
+      <c r="D170" s="22"/>
+      <c r="E170" s="22"/>
+      <c r="F170" s="22"/>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="24"/>
-      <c r="B171" s="24"/>
-      <c r="C171" s="24"/>
-      <c r="D171" s="25"/>
-      <c r="E171" s="25"/>
-      <c r="F171" s="25"/>
+      <c r="A171" s="21"/>
+      <c r="B171" s="21"/>
+      <c r="C171" s="21"/>
+      <c r="D171" s="22"/>
+      <c r="E171" s="22"/>
+      <c r="F171" s="22"/>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="24"/>
-      <c r="B172" s="24"/>
-      <c r="C172" s="24"/>
-      <c r="D172" s="25"/>
-      <c r="E172" s="25"/>
-      <c r="F172" s="25"/>
+      <c r="A172" s="21"/>
+      <c r="B172" s="21"/>
+      <c r="C172" s="21"/>
+      <c r="D172" s="22"/>
+      <c r="E172" s="22"/>
+      <c r="F172" s="22"/>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="24"/>
-      <c r="B173" s="24"/>
-      <c r="C173" s="24"/>
-      <c r="D173" s="25"/>
-      <c r="E173" s="25"/>
-      <c r="F173" s="25"/>
+      <c r="A173" s="21"/>
+      <c r="B173" s="21"/>
+      <c r="C173" s="21"/>
+      <c r="D173" s="22"/>
+      <c r="E173" s="22"/>
+      <c r="F173" s="22"/>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="24"/>
-      <c r="B174" s="24"/>
-      <c r="C174" s="24"/>
-      <c r="D174" s="25"/>
-      <c r="E174" s="25"/>
-      <c r="F174" s="25"/>
+      <c r="A174" s="21"/>
+      <c r="B174" s="21"/>
+      <c r="C174" s="21"/>
+      <c r="D174" s="22"/>
+      <c r="E174" s="22"/>
+      <c r="F174" s="22"/>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="24"/>
-      <c r="B175" s="24"/>
-      <c r="C175" s="24"/>
-      <c r="D175" s="25"/>
-      <c r="E175" s="25"/>
-      <c r="F175" s="25"/>
+      <c r="A175" s="21"/>
+      <c r="B175" s="21"/>
+      <c r="C175" s="21"/>
+      <c r="D175" s="22"/>
+      <c r="E175" s="22"/>
+      <c r="F175" s="22"/>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="24"/>
-      <c r="B176" s="24"/>
-      <c r="C176" s="24"/>
-      <c r="D176" s="25"/>
-      <c r="E176" s="25"/>
-      <c r="F176" s="25"/>
+      <c r="A176" s="21"/>
+      <c r="B176" s="21"/>
+      <c r="C176" s="21"/>
+      <c r="D176" s="22"/>
+      <c r="E176" s="22"/>
+      <c r="F176" s="22"/>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="24"/>
-      <c r="B177" s="24"/>
-      <c r="C177" s="24"/>
-      <c r="D177" s="25"/>
-      <c r="E177" s="25"/>
-      <c r="F177" s="25"/>
+      <c r="A177" s="21"/>
+      <c r="B177" s="21"/>
+      <c r="C177" s="21"/>
+      <c r="D177" s="22"/>
+      <c r="E177" s="22"/>
+      <c r="F177" s="22"/>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="24"/>
-      <c r="B178" s="24"/>
-      <c r="C178" s="24"/>
-      <c r="D178" s="25"/>
-      <c r="E178" s="25"/>
-      <c r="F178" s="25"/>
+      <c r="A178" s="21"/>
+      <c r="B178" s="21"/>
+      <c r="C178" s="21"/>
+      <c r="D178" s="22"/>
+      <c r="E178" s="22"/>
+      <c r="F178" s="22"/>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="24"/>
-      <c r="B179" s="24"/>
-      <c r="C179" s="24"/>
-      <c r="D179" s="25"/>
-      <c r="E179" s="25"/>
-      <c r="F179" s="25"/>
+      <c r="A179" s="21"/>
+      <c r="B179" s="21"/>
+      <c r="C179" s="21"/>
+      <c r="D179" s="22"/>
+      <c r="E179" s="22"/>
+      <c r="F179" s="22"/>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="24"/>
-      <c r="B180" s="24"/>
-      <c r="C180" s="24"/>
-      <c r="D180" s="25"/>
-      <c r="E180" s="25"/>
-      <c r="F180" s="25"/>
+      <c r="A180" s="21"/>
+      <c r="B180" s="21"/>
+      <c r="C180" s="21"/>
+      <c r="D180" s="22"/>
+      <c r="E180" s="22"/>
+      <c r="F180" s="22"/>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="24"/>
-      <c r="B181" s="24"/>
-      <c r="C181" s="24"/>
-      <c r="D181" s="25"/>
-      <c r="E181" s="25"/>
-      <c r="F181" s="25"/>
+      <c r="A181" s="21"/>
+      <c r="B181" s="21"/>
+      <c r="C181" s="21"/>
+      <c r="D181" s="22"/>
+      <c r="E181" s="22"/>
+      <c r="F181" s="22"/>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="24"/>
-      <c r="B182" s="24"/>
-      <c r="C182" s="24"/>
-      <c r="D182" s="25"/>
-      <c r="E182" s="25"/>
-      <c r="F182" s="25"/>
+      <c r="A182" s="21"/>
+      <c r="B182" s="21"/>
+      <c r="C182" s="21"/>
+      <c r="D182" s="22"/>
+      <c r="E182" s="22"/>
+      <c r="F182" s="22"/>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="24"/>
-      <c r="B183" s="24"/>
-      <c r="C183" s="24"/>
-      <c r="D183" s="25"/>
-      <c r="E183" s="25"/>
-      <c r="F183" s="25"/>
+      <c r="A183" s="21"/>
+      <c r="B183" s="21"/>
+      <c r="C183" s="21"/>
+      <c r="D183" s="22"/>
+      <c r="E183" s="22"/>
+      <c r="F183" s="22"/>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="24"/>
-      <c r="B184" s="24"/>
-      <c r="C184" s="24"/>
-      <c r="D184" s="25"/>
-      <c r="E184" s="25"/>
-      <c r="F184" s="25"/>
+      <c r="A184" s="21"/>
+      <c r="B184" s="21"/>
+      <c r="C184" s="21"/>
+      <c r="D184" s="22"/>
+      <c r="E184" s="22"/>
+      <c r="F184" s="22"/>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="24"/>
-      <c r="B185" s="24"/>
-      <c r="C185" s="24"/>
-      <c r="D185" s="25"/>
-      <c r="E185" s="25"/>
-      <c r="F185" s="25"/>
+      <c r="A185" s="21"/>
+      <c r="B185" s="21"/>
+      <c r="C185" s="21"/>
+      <c r="D185" s="22"/>
+      <c r="E185" s="22"/>
+      <c r="F185" s="22"/>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="24"/>
-      <c r="B186" s="24"/>
-      <c r="C186" s="24"/>
-      <c r="D186" s="25"/>
-      <c r="E186" s="25"/>
-      <c r="F186" s="25"/>
+      <c r="A186" s="21"/>
+      <c r="B186" s="21"/>
+      <c r="C186" s="21"/>
+      <c r="D186" s="22"/>
+      <c r="E186" s="22"/>
+      <c r="F186" s="22"/>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="24"/>
-      <c r="B187" s="24"/>
-      <c r="C187" s="24"/>
-      <c r="D187" s="25"/>
-      <c r="E187" s="25"/>
-      <c r="F187" s="25"/>
+      <c r="A187" s="21"/>
+      <c r="B187" s="21"/>
+      <c r="C187" s="21"/>
+      <c r="D187" s="22"/>
+      <c r="E187" s="22"/>
+      <c r="F187" s="22"/>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="24"/>
-      <c r="B188" s="24"/>
-      <c r="C188" s="24"/>
-      <c r="D188" s="25"/>
-      <c r="E188" s="25"/>
-      <c r="F188" s="25"/>
+      <c r="A188" s="21"/>
+      <c r="B188" s="21"/>
+      <c r="C188" s="21"/>
+      <c r="D188" s="22"/>
+      <c r="E188" s="22"/>
+      <c r="F188" s="22"/>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="24"/>
-      <c r="B189" s="24"/>
-      <c r="C189" s="24"/>
-      <c r="D189" s="25"/>
-      <c r="E189" s="25"/>
-      <c r="F189" s="25"/>
+      <c r="A189" s="21"/>
+      <c r="B189" s="21"/>
+      <c r="C189" s="21"/>
+      <c r="D189" s="22"/>
+      <c r="E189" s="22"/>
+      <c r="F189" s="22"/>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="24"/>
-      <c r="B190" s="24"/>
-      <c r="C190" s="24"/>
-      <c r="D190" s="25"/>
-      <c r="E190" s="25"/>
-      <c r="F190" s="25"/>
+      <c r="A190" s="21"/>
+      <c r="B190" s="21"/>
+      <c r="C190" s="21"/>
+      <c r="D190" s="22"/>
+      <c r="E190" s="22"/>
+      <c r="F190" s="22"/>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D191" s="3"/>

</xml_diff>